<commit_message>
Stuck on bind and case issues
I think we need to use typeCheck in Eval.hs. Have to resolve issues with bind and case syntax
</commit_message>
<xml_diff>
--- a/time-labor/week-of-06june2016.xlsx
+++ b/time-labor/week-of-06june2016.xlsx
@@ -26,6 +26,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -595,17 +596,17 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -855,16 +856,16 @@
         <v>25</v>
       </c>
       <c r="C15" s="19" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D15" s="20" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
         <f aca="false">IF((((D15-C15)+(F15-E15))*24)&gt;8,8,((D15-C15)+(F15-E15))*24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="21" t="n">
         <f aca="false">IF(((D15-C15)+(F15-E15))*24&gt;8,((D15-C15)+(F15-E15))*24-8,0)</f>
@@ -976,7 +977,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>12.8333333333333</v>
+        <v>15.8333333333333</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1020,7 +1021,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>128.333333333333</v>
+        <v>158.333333333333</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1036,7 +1037,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>128.333333333333</v>
+        <v>158.333333333333</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Building better test cases
Commiting to switch  workspaces, updating T/L.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-06june2016.xlsx
+++ b/time-labor/week-of-06june2016.xlsx
@@ -27,6 +27,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -596,17 +598,17 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -879,13 +881,17 @@
       <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="19" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D16" s="20" t="n">
+        <v>0.708333333333333</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -900,16 +906,16 @@
         <v>27</v>
       </c>
       <c r="C17" s="19" t="n">
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="D17" s="20" t="n">
-        <v>0</v>
+        <v>0.423611111111111</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>2.16666666666667</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -977,7 +983,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>15.8333333333333</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1021,7 +1027,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>158.333333333333</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1037,7 +1043,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>158.333333333333</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>